<commit_message>
updated table to read "initial probability"
</commit_message>
<xml_diff>
--- a/supplementary_table.xlsx
+++ b/supplementary_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturjaroszewicz/elab/HMX/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05B4B0BD-0C19-3948-9C35-AC484438937D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1279536-5208-B045-98AD-A1F221E63DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixture enrichments" sheetId="1" r:id="rId1"/>
@@ -391,16 +391,16 @@
     <t>Promoter Enrichment</t>
   </si>
   <si>
-    <t>Prior Probability</t>
-  </si>
-  <si>
-    <t>Prior Probability Given Mixture</t>
-  </si>
-  <si>
     <t>Mixture Number</t>
   </si>
   <si>
     <t>State From \ To</t>
+  </si>
+  <si>
+    <t>Initial Probability</t>
+  </si>
+  <si>
+    <t>Initial Probability Given Mixture</t>
   </si>
 </sst>
 </file>
@@ -696,10 +696,19 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,15 +737,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -959,7 +959,7 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -31438,11 +31438,11 @@
   </sheetPr>
   <dimension ref="A1:T999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -31507,17 +31507,17 @@
         <v>118</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="T1" s="27" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="62">
+      <c r="A2" s="65">
         <v>1</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="29">
@@ -31692,10 +31692,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="63">
+      <c r="A5" s="66">
         <v>2</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="63" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="35">
@@ -31870,10 +31870,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="64">
+      <c r="A8" s="67">
         <v>3</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="63" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="37">
@@ -32048,10 +32048,10 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="67">
+      <c r="A11" s="70">
         <v>4</v>
       </c>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="63" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="39">
@@ -32226,10 +32226,10 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="68">
+      <c r="A14" s="71">
         <v>5</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="63" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="41">
@@ -32404,10 +32404,10 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="69">
+      <c r="A17" s="72">
         <v>6</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="63" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="43">
@@ -32582,10 +32582,10 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="70">
+      <c r="A20" s="73">
         <v>7</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="63" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="45">
@@ -32760,10 +32760,10 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="71">
+      <c r="A23" s="59">
         <v>8</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C23" s="47">
@@ -32938,10 +32938,10 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="72">
+      <c r="A26" s="61">
         <v>9</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="63" t="s">
         <v>81</v>
       </c>
       <c r="C26" s="49">
@@ -33116,10 +33116,10 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="73">
+      <c r="A29" s="62">
         <v>10</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="63" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="51">
@@ -33294,10 +33294,10 @@
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="65">
+      <c r="A32" s="68">
         <v>11</v>
       </c>
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="63" t="s">
         <v>91</v>
       </c>
       <c r="C32" s="53">
@@ -33472,10 +33472,10 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="66">
+      <c r="A35" s="69">
         <v>12</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="64" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="55">
@@ -36537,11 +36537,9 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
@@ -36558,9 +36556,11 @@
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="D2:O37">
     <cfRule type="colorScale" priority="1">
@@ -36632,64 +36632,64 @@
       <c r="A1" s="34"/>
       <c r="B1" s="34"/>
       <c r="C1" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="62">
+        <v>119</v>
+      </c>
+      <c r="D1" s="65">
         <v>1</v>
       </c>
       <c r="E1" s="60"/>
       <c r="F1" s="60"/>
-      <c r="G1" s="63">
+      <c r="G1" s="66">
         <v>4</v>
       </c>
       <c r="H1" s="60"/>
       <c r="I1" s="60"/>
-      <c r="J1" s="64">
+      <c r="J1" s="67">
         <v>7</v>
       </c>
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
-      <c r="M1" s="67">
+      <c r="M1" s="70">
         <v>10</v>
       </c>
       <c r="N1" s="60"/>
       <c r="O1" s="60"/>
-      <c r="P1" s="68">
+      <c r="P1" s="71">
         <v>13</v>
       </c>
       <c r="Q1" s="60"/>
       <c r="R1" s="60"/>
-      <c r="S1" s="69">
+      <c r="S1" s="72">
         <v>16</v>
       </c>
       <c r="T1" s="60"/>
       <c r="U1" s="60"/>
-      <c r="V1" s="70">
+      <c r="V1" s="73">
         <v>19</v>
       </c>
       <c r="W1" s="60"/>
       <c r="X1" s="60"/>
-      <c r="Y1" s="71">
+      <c r="Y1" s="59">
         <v>22</v>
       </c>
       <c r="Z1" s="60"/>
       <c r="AA1" s="60"/>
-      <c r="AB1" s="72">
+      <c r="AB1" s="61">
         <v>25</v>
       </c>
       <c r="AC1" s="60"/>
       <c r="AD1" s="60"/>
-      <c r="AE1" s="73">
+      <c r="AE1" s="62">
         <v>28</v>
       </c>
       <c r="AF1" s="60"/>
       <c r="AG1" s="60"/>
-      <c r="AH1" s="65">
+      <c r="AH1" s="68">
         <v>31</v>
       </c>
       <c r="AI1" s="60"/>
       <c r="AJ1" s="60"/>
-      <c r="AK1" s="66">
+      <c r="AK1" s="69">
         <v>34</v>
       </c>
       <c r="AL1" s="60"/>
@@ -36701,62 +36701,62 @@
       <c r="C2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="63" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="63" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="60"/>
       <c r="I2" s="60"/>
-      <c r="J2" s="59" t="s">
+      <c r="J2" s="63" t="s">
         <v>51</v>
       </c>
       <c r="K2" s="60"/>
       <c r="L2" s="60"/>
-      <c r="M2" s="59" t="s">
+      <c r="M2" s="63" t="s">
         <v>56</v>
       </c>
       <c r="N2" s="60"/>
       <c r="O2" s="60"/>
-      <c r="P2" s="59" t="s">
+      <c r="P2" s="63" t="s">
         <v>61</v>
       </c>
       <c r="Q2" s="60"/>
       <c r="R2" s="60"/>
-      <c r="S2" s="59" t="s">
+      <c r="S2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="T2" s="60"/>
       <c r="U2" s="60"/>
-      <c r="V2" s="59" t="s">
+      <c r="V2" s="63" t="s">
         <v>71</v>
       </c>
       <c r="W2" s="60"/>
       <c r="X2" s="60"/>
-      <c r="Y2" s="59" t="s">
+      <c r="Y2" s="63" t="s">
         <v>76</v>
       </c>
       <c r="Z2" s="60"/>
       <c r="AA2" s="60"/>
-      <c r="AB2" s="59" t="s">
+      <c r="AB2" s="63" t="s">
         <v>81</v>
       </c>
       <c r="AC2" s="60"/>
       <c r="AD2" s="60"/>
-      <c r="AE2" s="59" t="s">
+      <c r="AE2" s="63" t="s">
         <v>86</v>
       </c>
       <c r="AF2" s="60"/>
       <c r="AG2" s="60"/>
-      <c r="AH2" s="59" t="s">
+      <c r="AH2" s="63" t="s">
         <v>91</v>
       </c>
       <c r="AI2" s="60"/>
       <c r="AJ2" s="60"/>
-      <c r="AK2" s="59" t="s">
+      <c r="AK2" s="63" t="s">
         <v>96</v>
       </c>
       <c r="AL2" s="60"/>
@@ -36770,7 +36770,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D3" s="28">
         <v>1</v>
@@ -36882,10 +36882,10 @@
       </c>
     </row>
     <row r="4" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="62">
+      <c r="A4" s="65">
         <v>1</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="28">
@@ -37231,10 +37231,10 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="63">
+      <c r="A7" s="66">
         <v>4</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="63" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="33">
@@ -37580,10 +37580,10 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="64">
+      <c r="A10" s="67">
         <v>7</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="63" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="36">
@@ -37929,10 +37929,10 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="67">
+      <c r="A13" s="70">
         <v>10</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="63" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="38">
@@ -38278,10 +38278,10 @@
       </c>
     </row>
     <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="68">
+      <c r="A16" s="71">
         <v>13</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="63" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="40">
@@ -38627,10 +38627,10 @@
       </c>
     </row>
     <row r="19" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="69">
+      <c r="A19" s="72">
         <v>16</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="63" t="s">
         <v>66</v>
       </c>
       <c r="C19" s="42">
@@ -38976,10 +38976,10 @@
       </c>
     </row>
     <row r="22" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="70">
+      <c r="A22" s="73">
         <v>19</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="63" t="s">
         <v>71</v>
       </c>
       <c r="C22" s="44">
@@ -39325,10 +39325,10 @@
       </c>
     </row>
     <row r="25" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="71">
+      <c r="A25" s="59">
         <v>22</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="46">
@@ -39674,10 +39674,10 @@
       </c>
     </row>
     <row r="28" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="72">
+      <c r="A28" s="61">
         <v>25</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="63" t="s">
         <v>81</v>
       </c>
       <c r="C28" s="48">
@@ -40023,10 +40023,10 @@
       </c>
     </row>
     <row r="31" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="73">
+      <c r="A31" s="62">
         <v>28</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="63" t="s">
         <v>86</v>
       </c>
       <c r="C31" s="50">
@@ -40372,10 +40372,10 @@
       </c>
     </row>
     <row r="34" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="65">
+      <c r="A34" s="68">
         <v>31</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="63" t="s">
         <v>91</v>
       </c>
       <c r="C34" s="52">
@@ -40721,10 +40721,10 @@
       </c>
     </row>
     <row r="37" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="66">
+      <c r="A37" s="69">
         <v>34</v>
       </c>
-      <c r="B37" s="61" t="s">
+      <c r="B37" s="64" t="s">
         <v>96</v>
       </c>
       <c r="C37" s="54">
@@ -41071,11 +41071,33 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:X2"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
@@ -41092,33 +41114,11 @@
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AD1"/>
-    <mergeCell ref="AE1:AG1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B34:B36"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:F6">
     <cfRule type="colorScale" priority="1">

</xml_diff>